<commit_message>
updated: data transfer now supports pcp model
</commit_message>
<xml_diff>
--- a/PropProAssistant/Models/BNC/BNC_01.xlsx
+++ b/PropProAssistant/Models/BNC/BNC_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Lote</t>
   </si>
@@ -42,6 +42,57 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Farmace</t>
+  </si>
+  <si>
+    <t>Hipolabor</t>
+  </si>
+  <si>
+    <t>Hypofarma</t>
+  </si>
+  <si>
+    <t>Isofarma</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>Teuto</t>
+  </si>
+  <si>
+    <t>Blau</t>
+  </si>
+  <si>
+    <t>Sanval</t>
+  </si>
+  <si>
+    <t>Cristália</t>
+  </si>
+  <si>
+    <t>Takeda</t>
+  </si>
+  <si>
+    <t>Mylan</t>
+  </si>
+  <si>
+    <t>Halex Istar</t>
+  </si>
+  <si>
+    <t>Belfar</t>
+  </si>
+  <si>
+    <t>Nativita</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>União Química</t>
+  </si>
+  <si>
+    <t>Eurofarma</t>
   </si>
 </sst>
 </file>
@@ -972,14 +1023,14 @@
       <c r="B5" s="0">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+      <c r="C5" s="1">
+        <v>4.42</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -989,14 +1040,14 @@
       <c r="B6" s="0">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
+      <c r="C6" s="1">
+        <v>7.15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -1006,14 +1057,14 @@
       <c r="B7" s="0">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
+      <c r="C7" s="1">
+        <v>2.99</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -1023,14 +1074,14 @@
       <c r="B8" s="0">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
+      <c r="C8" s="1">
+        <v>0.65</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -1057,14 +1108,14 @@
       <c r="B10" s="0">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
+      <c r="C10" s="1">
+        <v>12.87</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -1074,14 +1125,14 @@
       <c r="B11" s="0">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
+      <c r="C11" s="1">
+        <v>76.7</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1244,14 +1295,14 @@
       <c r="B21" s="0">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
+      <c r="C21" s="1">
+        <v>12.35</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -1346,14 +1397,14 @@
       <c r="B27" s="0">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
+      <c r="C27" s="1">
+        <v>3.38</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1482,14 +1533,14 @@
       <c r="B35" s="0">
         <v>34</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
+      <c r="C35" s="1">
+        <v>8.97</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
@@ -1499,14 +1550,14 @@
       <c r="B36" s="0">
         <v>35</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
+      <c r="C36" s="1">
+        <v>17.55</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
@@ -1516,14 +1567,14 @@
       <c r="B37" s="0">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
+      <c r="C37" s="1">
+        <v>6.37</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
@@ -1584,14 +1635,14 @@
       <c r="B41" s="0">
         <v>40</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>5</v>
+      <c r="C41" s="1">
+        <v>3.25</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -1618,14 +1669,14 @@
       <c r="B43" s="0">
         <v>42</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>5</v>
+      <c r="C43" s="1">
+        <v>44.2</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
@@ -1958,14 +2009,14 @@
       <c r="B63" s="0">
         <v>62</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>5</v>
+      <c r="C63" s="1">
+        <v>3.9</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64">
@@ -1975,14 +2026,14 @@
       <c r="B64" s="0">
         <v>63</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>5</v>
+      <c r="C64" s="1">
+        <v>10.4</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65">
@@ -2009,14 +2060,14 @@
       <c r="B66" s="0">
         <v>65</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>5</v>
+      <c r="C66" s="1">
+        <v>3.51</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67">
@@ -2094,14 +2145,14 @@
       <c r="B71" s="0">
         <v>70</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>5</v>
+      <c r="C71" s="1">
+        <v>1.95</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
@@ -2128,14 +2179,14 @@
       <c r="B73" s="0">
         <v>72</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>5</v>
+      <c r="C73" s="1">
+        <v>24.7</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
@@ -2162,14 +2213,14 @@
       <c r="B75" s="0">
         <v>74</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>5</v>
+      <c r="C75" s="1">
+        <v>2.08</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76">
@@ -2264,14 +2315,14 @@
       <c r="B81" s="0">
         <v>80</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>5</v>
+      <c r="C81" s="1">
+        <v>89.7</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82">
@@ -2281,14 +2332,14 @@
       <c r="B82" s="0">
         <v>81</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>5</v>
+      <c r="C82" s="1">
+        <v>29.9</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83">
@@ -2451,14 +2502,14 @@
       <c r="B92" s="0">
         <v>91</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>5</v>
+      <c r="C92" s="1">
+        <v>7.15</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
@@ -2485,14 +2536,14 @@
       <c r="B94" s="0">
         <v>93</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>5</v>
+      <c r="C94" s="1">
+        <v>2.47</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95">
@@ -2587,14 +2638,14 @@
       <c r="B100" s="0">
         <v>99</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>5</v>
+      <c r="C100" s="1">
+        <v>1.24</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101">
@@ -2638,14 +2689,14 @@
       <c r="B103" s="0">
         <v>102</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>5</v>
+      <c r="C103" s="1">
+        <v>11.57</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104">
@@ -2706,14 +2757,14 @@
       <c r="B107" s="0">
         <v>106</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>5</v>
+      <c r="C107" s="1">
+        <v>6.37</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108">
@@ -2723,14 +2774,14 @@
       <c r="B108" s="0">
         <v>107</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>5</v>
+      <c r="C108" s="1">
+        <v>9.09</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109">
@@ -2978,14 +3029,14 @@
       <c r="B123" s="0">
         <v>122</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>5</v>
+      <c r="C123" s="1">
+        <v>8.97</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124">
@@ -3165,14 +3216,14 @@
       <c r="B134" s="0">
         <v>133</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>5</v>
+      <c r="C134" s="1">
+        <v>12.09</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135">
@@ -3199,14 +3250,14 @@
       <c r="B136" s="0">
         <v>135</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>5</v>
+      <c r="C136" s="1">
+        <v>3.77</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137">
@@ -3301,14 +3352,14 @@
       <c r="B142" s="0">
         <v>141</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>5</v>
+      <c r="C142" s="1">
+        <v>36.4</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143">
@@ -3318,14 +3369,14 @@
       <c r="B143" s="0">
         <v>142</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>5</v>
+      <c r="C143" s="1">
+        <v>3.89</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144">
@@ -3335,14 +3386,14 @@
       <c r="B144" s="0">
         <v>143</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>5</v>
+      <c r="C144" s="1">
+        <v>20.8</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145">
@@ -3352,14 +3403,14 @@
       <c r="B145" s="0">
         <v>144</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>5</v>
+      <c r="C145" s="1">
+        <v>4</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="146">
@@ -3369,14 +3420,14 @@
       <c r="B146" s="0">
         <v>145</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>5</v>
+      <c r="C146" s="1">
+        <v>14.82</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147">
@@ -3522,14 +3573,14 @@
       <c r="B155" s="0">
         <v>154</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>5</v>
+      <c r="C155" s="1">
+        <v>12.35</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156">
@@ -3539,14 +3590,14 @@
       <c r="B156" s="0">
         <v>155</v>
       </c>
-      <c r="C156" s="1" t="s">
-        <v>5</v>
+      <c r="C156" s="1">
+        <v>8.32</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157">
@@ -3556,14 +3607,14 @@
       <c r="B157" s="0">
         <v>156</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>5</v>
+      <c r="C157" s="1">
+        <v>9.36</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158">
@@ -3573,14 +3624,14 @@
       <c r="B158" s="0">
         <v>157</v>
       </c>
-      <c r="C158" s="1" t="s">
-        <v>5</v>
+      <c r="C158" s="1">
+        <v>9.88</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159">
@@ -3590,14 +3641,14 @@
       <c r="B159" s="0">
         <v>158</v>
       </c>
-      <c r="C159" s="1" t="s">
-        <v>5</v>
+      <c r="C159" s="1">
+        <v>14.17</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="160">
@@ -3607,14 +3658,14 @@
       <c r="B160" s="0">
         <v>159</v>
       </c>
-      <c r="C160" s="1" t="s">
-        <v>5</v>
+      <c r="C160" s="1">
+        <v>12.87</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161">
@@ -3658,14 +3709,14 @@
       <c r="B163" s="0">
         <v>162</v>
       </c>
-      <c r="C163" s="1" t="s">
-        <v>5</v>
+      <c r="C163" s="1">
+        <v>12.87</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164">
@@ -3675,14 +3726,14 @@
       <c r="B164" s="0">
         <v>163</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>5</v>
+      <c r="C164" s="1">
+        <v>3.77</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165">
@@ -3777,14 +3828,14 @@
       <c r="B170" s="0">
         <v>169</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>5</v>
+      <c r="C170" s="1">
+        <v>21.48</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E170" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171">
@@ -3811,14 +3862,14 @@
       <c r="B172" s="0">
         <v>171</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>5</v>
+      <c r="C172" s="1">
+        <v>11.7</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173">
@@ -3845,14 +3896,14 @@
       <c r="B174" s="0">
         <v>173</v>
       </c>
-      <c r="C174" s="1" t="s">
-        <v>5</v>
+      <c r="C174" s="1">
+        <v>3.25</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175">
@@ -3998,14 +4049,14 @@
       <c r="B183" s="0">
         <v>182</v>
       </c>
-      <c r="C183" s="1" t="s">
-        <v>5</v>
+      <c r="C183" s="1">
+        <v>2.08</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184">
@@ -4032,14 +4083,14 @@
       <c r="B185" s="0">
         <v>184</v>
       </c>
-      <c r="C185" s="1" t="s">
-        <v>5</v>
+      <c r="C185" s="1">
+        <v>23.4</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186">
@@ -4134,14 +4185,14 @@
       <c r="B191" s="0">
         <v>190</v>
       </c>
-      <c r="C191" s="1" t="s">
-        <v>5</v>
+      <c r="C191" s="1">
+        <v>14.3</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E191" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192">
@@ -4151,14 +4202,14 @@
       <c r="B192" s="0">
         <v>191</v>
       </c>
-      <c r="C192" s="1" t="s">
-        <v>5</v>
+      <c r="C192" s="1">
+        <v>7.67</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E192" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="193">
@@ -4219,14 +4270,14 @@
       <c r="B196" s="0">
         <v>195</v>
       </c>
-      <c r="C196" s="1" t="s">
-        <v>5</v>
+      <c r="C196" s="1">
+        <v>11.7</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E196" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="197">

</xml_diff>

<commit_message>
fix: resets the value of items missing from the proposal
</commit_message>
<xml_diff>
--- a/PropProAssistant/Models/BNC/BNC_01.xlsx
+++ b/PropProAssistant/Models/BNC/BNC_01.xlsx
@@ -972,8 +972,8 @@
       <c r="B2" s="0">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="1">
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>5</v>
@@ -989,8 +989,8 @@
       <c r="B3" s="0">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="1">
+        <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>5</v>
@@ -1006,8 +1006,8 @@
       <c r="B4" s="0">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
+      <c r="C4" s="1">
+        <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>5</v>
@@ -1091,8 +1091,8 @@
       <c r="B9" s="0">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
+      <c r="C9" s="1">
+        <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>5</v>
@@ -1142,8 +1142,8 @@
       <c r="B12" s="0">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
+      <c r="C12" s="1">
+        <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>5</v>
@@ -1159,8 +1159,8 @@
       <c r="B13" s="0">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
+      <c r="C13" s="1">
+        <v>0</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>5</v>
@@ -1176,8 +1176,8 @@
       <c r="B14" s="0">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
+      <c r="C14" s="1">
+        <v>0</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>5</v>
@@ -1193,8 +1193,8 @@
       <c r="B15" s="0">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
+      <c r="C15" s="1">
+        <v>0</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>5</v>
@@ -1210,8 +1210,8 @@
       <c r="B16" s="0">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
+      <c r="C16" s="1">
+        <v>0</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>5</v>
@@ -1227,8 +1227,8 @@
       <c r="B17" s="0">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
+      <c r="C17" s="1">
+        <v>0</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>5</v>
@@ -1244,8 +1244,8 @@
       <c r="B18" s="0">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
+      <c r="C18" s="1">
+        <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>5</v>
@@ -1261,8 +1261,8 @@
       <c r="B19" s="0">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
+      <c r="C19" s="1">
+        <v>0</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>5</v>
@@ -1278,8 +1278,8 @@
       <c r="B20" s="0">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
+      <c r="C20" s="1">
+        <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>5</v>
@@ -1312,8 +1312,8 @@
       <c r="B22" s="0">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
+      <c r="C22" s="1">
+        <v>0</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>5</v>
@@ -1329,8 +1329,8 @@
       <c r="B23" s="0">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
+      <c r="C23" s="1">
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>5</v>
@@ -1346,8 +1346,8 @@
       <c r="B24" s="0">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
+      <c r="C24" s="1">
+        <v>0</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>5</v>
@@ -1363,8 +1363,8 @@
       <c r="B25" s="0">
         <v>24</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
+      <c r="C25" s="1">
+        <v>0</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>5</v>
@@ -1380,8 +1380,8 @@
       <c r="B26" s="0">
         <v>25</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
+      <c r="C26" s="1">
+        <v>0</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>5</v>
@@ -1414,8 +1414,8 @@
       <c r="B28" s="0">
         <v>27</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
+      <c r="C28" s="1">
+        <v>0</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>5</v>
@@ -1431,8 +1431,8 @@
       <c r="B29" s="0">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
+      <c r="C29" s="1">
+        <v>0</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>5</v>
@@ -1448,8 +1448,8 @@
       <c r="B30" s="0">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
+      <c r="C30" s="1">
+        <v>0</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>5</v>
@@ -1465,8 +1465,8 @@
       <c r="B31" s="0">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
+      <c r="C31" s="1">
+        <v>0</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>5</v>
@@ -1482,8 +1482,8 @@
       <c r="B32" s="0">
         <v>31</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
+      <c r="C32" s="1">
+        <v>0</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>5</v>
@@ -1499,8 +1499,8 @@
       <c r="B33" s="0">
         <v>32</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
+      <c r="C33" s="1">
+        <v>0</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>5</v>
@@ -1516,8 +1516,8 @@
       <c r="B34" s="0">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
+      <c r="C34" s="1">
+        <v>0</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>5</v>
@@ -1584,8 +1584,8 @@
       <c r="B38" s="0">
         <v>37</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
+      <c r="C38" s="1">
+        <v>0</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>5</v>
@@ -1601,8 +1601,8 @@
       <c r="B39" s="0">
         <v>38</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
+      <c r="C39" s="1">
+        <v>0</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>5</v>
@@ -1618,8 +1618,8 @@
       <c r="B40" s="0">
         <v>39</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>5</v>
+      <c r="C40" s="1">
+        <v>0</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>5</v>
@@ -1652,8 +1652,8 @@
       <c r="B42" s="0">
         <v>41</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>5</v>
+      <c r="C42" s="1">
+        <v>0</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>5</v>
@@ -1686,8 +1686,8 @@
       <c r="B44" s="0">
         <v>43</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>5</v>
+      <c r="C44" s="1">
+        <v>0</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>5</v>
@@ -1703,8 +1703,8 @@
       <c r="B45" s="0">
         <v>44</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>5</v>
+      <c r="C45" s="1">
+        <v>0</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>5</v>
@@ -1720,8 +1720,8 @@
       <c r="B46" s="0">
         <v>45</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>5</v>
+      <c r="C46" s="1">
+        <v>0</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>5</v>
@@ -1737,8 +1737,8 @@
       <c r="B47" s="0">
         <v>46</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>5</v>
+      <c r="C47" s="1">
+        <v>0</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>5</v>
@@ -1754,8 +1754,8 @@
       <c r="B48" s="0">
         <v>47</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>5</v>
+      <c r="C48" s="1">
+        <v>0</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>5</v>
@@ -1771,8 +1771,8 @@
       <c r="B49" s="0">
         <v>48</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
+      <c r="C49" s="1">
+        <v>0</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>5</v>
@@ -1788,8 +1788,8 @@
       <c r="B50" s="0">
         <v>49</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>5</v>
+      <c r="C50" s="1">
+        <v>0</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>5</v>
@@ -1805,8 +1805,8 @@
       <c r="B51" s="0">
         <v>50</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>5</v>
+      <c r="C51" s="1">
+        <v>0</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>5</v>
@@ -1822,8 +1822,8 @@
       <c r="B52" s="0">
         <v>51</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>5</v>
+      <c r="C52" s="1">
+        <v>0</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>5</v>
@@ -1839,8 +1839,8 @@
       <c r="B53" s="0">
         <v>52</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>5</v>
+      <c r="C53" s="1">
+        <v>0</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>5</v>
@@ -1856,8 +1856,8 @@
       <c r="B54" s="0">
         <v>53</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>5</v>
+      <c r="C54" s="1">
+        <v>0</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>5</v>
@@ -1873,8 +1873,8 @@
       <c r="B55" s="0">
         <v>54</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>5</v>
+      <c r="C55" s="1">
+        <v>0</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>5</v>
@@ -1890,8 +1890,8 @@
       <c r="B56" s="0">
         <v>55</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>5</v>
+      <c r="C56" s="1">
+        <v>0</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>5</v>
@@ -1907,8 +1907,8 @@
       <c r="B57" s="0">
         <v>56</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
+      <c r="C57" s="1">
+        <v>0</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>5</v>
@@ -1924,8 +1924,8 @@
       <c r="B58" s="0">
         <v>57</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
+      <c r="C58" s="1">
+        <v>0</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>5</v>
@@ -1941,8 +1941,8 @@
       <c r="B59" s="0">
         <v>58</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
+      <c r="C59" s="1">
+        <v>0</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>5</v>
@@ -1958,8 +1958,8 @@
       <c r="B60" s="0">
         <v>59</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
+      <c r="C60" s="1">
+        <v>0</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>5</v>
@@ -1975,8 +1975,8 @@
       <c r="B61" s="0">
         <v>60</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>5</v>
+      <c r="C61" s="1">
+        <v>0</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>5</v>
@@ -1992,8 +1992,8 @@
       <c r="B62" s="0">
         <v>61</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>5</v>
+      <c r="C62" s="1">
+        <v>0</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>5</v>
@@ -2043,8 +2043,8 @@
       <c r="B65" s="0">
         <v>64</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>5</v>
+      <c r="C65" s="1">
+        <v>0</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>5</v>
@@ -2077,8 +2077,8 @@
       <c r="B67" s="0">
         <v>66</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>5</v>
+      <c r="C67" s="1">
+        <v>0</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>5</v>
@@ -2094,8 +2094,8 @@
       <c r="B68" s="0">
         <v>67</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>5</v>
+      <c r="C68" s="1">
+        <v>0</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>5</v>
@@ -2111,8 +2111,8 @@
       <c r="B69" s="0">
         <v>68</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>5</v>
+      <c r="C69" s="1">
+        <v>0</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>5</v>
@@ -2128,8 +2128,8 @@
       <c r="B70" s="0">
         <v>69</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>5</v>
+      <c r="C70" s="1">
+        <v>0</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>5</v>
@@ -2162,8 +2162,8 @@
       <c r="B72" s="0">
         <v>71</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>5</v>
+      <c r="C72" s="1">
+        <v>0</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>5</v>
@@ -2196,8 +2196,8 @@
       <c r="B74" s="0">
         <v>73</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>5</v>
+      <c r="C74" s="1">
+        <v>0</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>5</v>
@@ -2230,8 +2230,8 @@
       <c r="B76" s="0">
         <v>75</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>5</v>
+      <c r="C76" s="1">
+        <v>0</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>5</v>
@@ -2247,8 +2247,8 @@
       <c r="B77" s="0">
         <v>76</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>5</v>
+      <c r="C77" s="1">
+        <v>0</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>5</v>
@@ -2264,8 +2264,8 @@
       <c r="B78" s="0">
         <v>77</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>5</v>
+      <c r="C78" s="1">
+        <v>0</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>5</v>
@@ -2281,8 +2281,8 @@
       <c r="B79" s="0">
         <v>78</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>5</v>
+      <c r="C79" s="1">
+        <v>0</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>5</v>
@@ -2298,8 +2298,8 @@
       <c r="B80" s="0">
         <v>79</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>5</v>
+      <c r="C80" s="1">
+        <v>0</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>5</v>
@@ -2349,8 +2349,8 @@
       <c r="B83" s="0">
         <v>82</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>5</v>
+      <c r="C83" s="1">
+        <v>0</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>5</v>
@@ -2366,8 +2366,8 @@
       <c r="B84" s="0">
         <v>83</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>5</v>
+      <c r="C84" s="1">
+        <v>0</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>5</v>
@@ -2383,8 +2383,8 @@
       <c r="B85" s="0">
         <v>84</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>5</v>
+      <c r="C85" s="1">
+        <v>0</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>5</v>
@@ -2400,8 +2400,8 @@
       <c r="B86" s="0">
         <v>85</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>5</v>
+      <c r="C86" s="1">
+        <v>0</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>5</v>
@@ -2417,8 +2417,8 @@
       <c r="B87" s="0">
         <v>86</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>5</v>
+      <c r="C87" s="1">
+        <v>0</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>5</v>
@@ -2434,8 +2434,8 @@
       <c r="B88" s="0">
         <v>87</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>5</v>
+      <c r="C88" s="1">
+        <v>0</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>5</v>
@@ -2451,8 +2451,8 @@
       <c r="B89" s="0">
         <v>88</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>5</v>
+      <c r="C89" s="1">
+        <v>0</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>5</v>
@@ -2468,8 +2468,8 @@
       <c r="B90" s="0">
         <v>89</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>5</v>
+      <c r="C90" s="1">
+        <v>0</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>5</v>
@@ -2485,8 +2485,8 @@
       <c r="B91" s="0">
         <v>90</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>5</v>
+      <c r="C91" s="1">
+        <v>0</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>5</v>
@@ -2519,8 +2519,8 @@
       <c r="B93" s="0">
         <v>92</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>5</v>
+      <c r="C93" s="1">
+        <v>0</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>5</v>
@@ -2553,8 +2553,8 @@
       <c r="B95" s="0">
         <v>94</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>5</v>
+      <c r="C95" s="1">
+        <v>0</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>5</v>
@@ -2570,8 +2570,8 @@
       <c r="B96" s="0">
         <v>95</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>5</v>
+      <c r="C96" s="1">
+        <v>0</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>5</v>
@@ -2587,8 +2587,8 @@
       <c r="B97" s="0">
         <v>96</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>5</v>
+      <c r="C97" s="1">
+        <v>0</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>5</v>
@@ -2604,8 +2604,8 @@
       <c r="B98" s="0">
         <v>97</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>5</v>
+      <c r="C98" s="1">
+        <v>0</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>5</v>
@@ -2621,8 +2621,8 @@
       <c r="B99" s="0">
         <v>98</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>5</v>
+      <c r="C99" s="1">
+        <v>0</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>5</v>
@@ -2655,8 +2655,8 @@
       <c r="B101" s="0">
         <v>100</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>5</v>
+      <c r="C101" s="1">
+        <v>0</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>5</v>
@@ -2672,8 +2672,8 @@
       <c r="B102" s="0">
         <v>101</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>5</v>
+      <c r="C102" s="1">
+        <v>0</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>5</v>
@@ -2706,8 +2706,8 @@
       <c r="B104" s="0">
         <v>103</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>5</v>
+      <c r="C104" s="1">
+        <v>0</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>5</v>
@@ -2723,8 +2723,8 @@
       <c r="B105" s="0">
         <v>104</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>5</v>
+      <c r="C105" s="1">
+        <v>0</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>5</v>
@@ -2740,8 +2740,8 @@
       <c r="B106" s="0">
         <v>105</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>5</v>
+      <c r="C106" s="1">
+        <v>0</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>5</v>
@@ -2791,8 +2791,8 @@
       <c r="B109" s="0">
         <v>108</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>5</v>
+      <c r="C109" s="1">
+        <v>0</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>5</v>
@@ -2808,8 +2808,8 @@
       <c r="B110" s="0">
         <v>109</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>5</v>
+      <c r="C110" s="1">
+        <v>0</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>5</v>
@@ -2825,8 +2825,8 @@
       <c r="B111" s="0">
         <v>110</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>5</v>
+      <c r="C111" s="1">
+        <v>0</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>5</v>
@@ -2842,8 +2842,8 @@
       <c r="B112" s="0">
         <v>111</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>5</v>
+      <c r="C112" s="1">
+        <v>0</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>5</v>
@@ -2859,8 +2859,8 @@
       <c r="B113" s="0">
         <v>112</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>5</v>
+      <c r="C113" s="1">
+        <v>0</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>5</v>
@@ -2876,8 +2876,8 @@
       <c r="B114" s="0">
         <v>113</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
+      <c r="C114" s="1">
+        <v>0</v>
       </c>
       <c r="D114" s="0" t="s">
         <v>5</v>
@@ -2893,8 +2893,8 @@
       <c r="B115" s="0">
         <v>114</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>5</v>
+      <c r="C115" s="1">
+        <v>0</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>5</v>
@@ -2910,8 +2910,8 @@
       <c r="B116" s="0">
         <v>115</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>5</v>
+      <c r="C116" s="1">
+        <v>0</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>5</v>
@@ -2927,8 +2927,8 @@
       <c r="B117" s="0">
         <v>116</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>5</v>
+      <c r="C117" s="1">
+        <v>0</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>5</v>
@@ -2944,8 +2944,8 @@
       <c r="B118" s="0">
         <v>117</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>5</v>
+      <c r="C118" s="1">
+        <v>0</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>5</v>
@@ -2961,8 +2961,8 @@
       <c r="B119" s="0">
         <v>118</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>5</v>
+      <c r="C119" s="1">
+        <v>0</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>5</v>
@@ -2978,8 +2978,8 @@
       <c r="B120" s="0">
         <v>119</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>5</v>
+      <c r="C120" s="1">
+        <v>0</v>
       </c>
       <c r="D120" s="0" t="s">
         <v>5</v>
@@ -2995,8 +2995,8 @@
       <c r="B121" s="0">
         <v>120</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>5</v>
+      <c r="C121" s="1">
+        <v>0</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>5</v>
@@ -3012,8 +3012,8 @@
       <c r="B122" s="0">
         <v>121</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>5</v>
+      <c r="C122" s="1">
+        <v>0</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>5</v>
@@ -3046,8 +3046,8 @@
       <c r="B124" s="0">
         <v>123</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>5</v>
+      <c r="C124" s="1">
+        <v>0</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>5</v>
@@ -3063,8 +3063,8 @@
       <c r="B125" s="0">
         <v>124</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>5</v>
+      <c r="C125" s="1">
+        <v>0</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>5</v>
@@ -3080,8 +3080,8 @@
       <c r="B126" s="0">
         <v>125</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>5</v>
+      <c r="C126" s="1">
+        <v>0</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>5</v>
@@ -3097,8 +3097,8 @@
       <c r="B127" s="0">
         <v>126</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>5</v>
+      <c r="C127" s="1">
+        <v>0</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>5</v>
@@ -3114,8 +3114,8 @@
       <c r="B128" s="0">
         <v>127</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>5</v>
+      <c r="C128" s="1">
+        <v>0</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>5</v>
@@ -3131,8 +3131,8 @@
       <c r="B129" s="0">
         <v>128</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>5</v>
+      <c r="C129" s="1">
+        <v>0</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>5</v>
@@ -3148,8 +3148,8 @@
       <c r="B130" s="0">
         <v>129</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>5</v>
+      <c r="C130" s="1">
+        <v>0</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>5</v>
@@ -3165,8 +3165,8 @@
       <c r="B131" s="0">
         <v>130</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>5</v>
+      <c r="C131" s="1">
+        <v>0</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>5</v>
@@ -3182,8 +3182,8 @@
       <c r="B132" s="0">
         <v>131</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>5</v>
+      <c r="C132" s="1">
+        <v>0</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>5</v>
@@ -3199,8 +3199,8 @@
       <c r="B133" s="0">
         <v>132</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>5</v>
+      <c r="C133" s="1">
+        <v>0</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>5</v>
@@ -3233,8 +3233,8 @@
       <c r="B135" s="0">
         <v>134</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>5</v>
+      <c r="C135" s="1">
+        <v>0</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>5</v>
@@ -3267,8 +3267,8 @@
       <c r="B137" s="0">
         <v>136</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>5</v>
+      <c r="C137" s="1">
+        <v>0</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>5</v>
@@ -3284,8 +3284,8 @@
       <c r="B138" s="0">
         <v>137</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>5</v>
+      <c r="C138" s="1">
+        <v>0</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>5</v>
@@ -3301,8 +3301,8 @@
       <c r="B139" s="0">
         <v>138</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>5</v>
+      <c r="C139" s="1">
+        <v>0</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>5</v>
@@ -3318,8 +3318,8 @@
       <c r="B140" s="0">
         <v>139</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>5</v>
+      <c r="C140" s="1">
+        <v>0</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>5</v>
@@ -3335,8 +3335,8 @@
       <c r="B141" s="0">
         <v>140</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>5</v>
+      <c r="C141" s="1">
+        <v>0</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>5</v>
@@ -3437,8 +3437,8 @@
       <c r="B147" s="0">
         <v>146</v>
       </c>
-      <c r="C147" s="1" t="s">
-        <v>5</v>
+      <c r="C147" s="1">
+        <v>0</v>
       </c>
       <c r="D147" s="0" t="s">
         <v>5</v>
@@ -3454,8 +3454,8 @@
       <c r="B148" s="0">
         <v>147</v>
       </c>
-      <c r="C148" s="1" t="s">
-        <v>5</v>
+      <c r="C148" s="1">
+        <v>0</v>
       </c>
       <c r="D148" s="0" t="s">
         <v>5</v>
@@ -3471,8 +3471,8 @@
       <c r="B149" s="0">
         <v>148</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>5</v>
+      <c r="C149" s="1">
+        <v>0</v>
       </c>
       <c r="D149" s="0" t="s">
         <v>5</v>
@@ -3488,8 +3488,8 @@
       <c r="B150" s="0">
         <v>149</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>5</v>
+      <c r="C150" s="1">
+        <v>0</v>
       </c>
       <c r="D150" s="0" t="s">
         <v>5</v>
@@ -3505,8 +3505,8 @@
       <c r="B151" s="0">
         <v>150</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>5</v>
+      <c r="C151" s="1">
+        <v>0</v>
       </c>
       <c r="D151" s="0" t="s">
         <v>5</v>
@@ -3522,8 +3522,8 @@
       <c r="B152" s="0">
         <v>151</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>5</v>
+      <c r="C152" s="1">
+        <v>0</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>5</v>
@@ -3539,8 +3539,8 @@
       <c r="B153" s="0">
         <v>152</v>
       </c>
-      <c r="C153" s="1" t="s">
-        <v>5</v>
+      <c r="C153" s="1">
+        <v>0</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>5</v>
@@ -3556,8 +3556,8 @@
       <c r="B154" s="0">
         <v>153</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>5</v>
+      <c r="C154" s="1">
+        <v>0</v>
       </c>
       <c r="D154" s="0" t="s">
         <v>5</v>
@@ -3675,8 +3675,8 @@
       <c r="B161" s="0">
         <v>160</v>
       </c>
-      <c r="C161" s="1" t="s">
-        <v>5</v>
+      <c r="C161" s="1">
+        <v>0</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>5</v>
@@ -3692,8 +3692,8 @@
       <c r="B162" s="0">
         <v>161</v>
       </c>
-      <c r="C162" s="1" t="s">
-        <v>5</v>
+      <c r="C162" s="1">
+        <v>0</v>
       </c>
       <c r="D162" s="0" t="s">
         <v>5</v>
@@ -3743,8 +3743,8 @@
       <c r="B165" s="0">
         <v>164</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>5</v>
+      <c r="C165" s="1">
+        <v>0</v>
       </c>
       <c r="D165" s="0" t="s">
         <v>5</v>
@@ -3760,8 +3760,8 @@
       <c r="B166" s="0">
         <v>165</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>5</v>
+      <c r="C166" s="1">
+        <v>0</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>5</v>
@@ -3777,8 +3777,8 @@
       <c r="B167" s="0">
         <v>166</v>
       </c>
-      <c r="C167" s="1" t="s">
-        <v>5</v>
+      <c r="C167" s="1">
+        <v>0</v>
       </c>
       <c r="D167" s="0" t="s">
         <v>5</v>
@@ -3794,8 +3794,8 @@
       <c r="B168" s="0">
         <v>167</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>5</v>
+      <c r="C168" s="1">
+        <v>0</v>
       </c>
       <c r="D168" s="0" t="s">
         <v>5</v>
@@ -3811,8 +3811,8 @@
       <c r="B169" s="0">
         <v>168</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>5</v>
+      <c r="C169" s="1">
+        <v>0</v>
       </c>
       <c r="D169" s="0" t="s">
         <v>5</v>
@@ -3845,8 +3845,8 @@
       <c r="B171" s="0">
         <v>170</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>5</v>
+      <c r="C171" s="1">
+        <v>0</v>
       </c>
       <c r="D171" s="0" t="s">
         <v>5</v>
@@ -3879,8 +3879,8 @@
       <c r="B173" s="0">
         <v>172</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>5</v>
+      <c r="C173" s="1">
+        <v>0</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>5</v>
@@ -3913,8 +3913,8 @@
       <c r="B175" s="0">
         <v>174</v>
       </c>
-      <c r="C175" s="1" t="s">
-        <v>5</v>
+      <c r="C175" s="1">
+        <v>0</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>5</v>
@@ -3930,8 +3930,8 @@
       <c r="B176" s="0">
         <v>175</v>
       </c>
-      <c r="C176" s="1" t="s">
-        <v>5</v>
+      <c r="C176" s="1">
+        <v>0</v>
       </c>
       <c r="D176" s="0" t="s">
         <v>5</v>
@@ -3947,8 +3947,8 @@
       <c r="B177" s="0">
         <v>176</v>
       </c>
-      <c r="C177" s="1" t="s">
-        <v>5</v>
+      <c r="C177" s="1">
+        <v>0</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>5</v>
@@ -3964,8 +3964,8 @@
       <c r="B178" s="0">
         <v>177</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>5</v>
+      <c r="C178" s="1">
+        <v>0</v>
       </c>
       <c r="D178" s="0" t="s">
         <v>5</v>
@@ -3981,8 +3981,8 @@
       <c r="B179" s="0">
         <v>178</v>
       </c>
-      <c r="C179" s="1" t="s">
-        <v>5</v>
+      <c r="C179" s="1">
+        <v>0</v>
       </c>
       <c r="D179" s="0" t="s">
         <v>5</v>
@@ -3998,8 +3998,8 @@
       <c r="B180" s="0">
         <v>179</v>
       </c>
-      <c r="C180" s="1" t="s">
-        <v>5</v>
+      <c r="C180" s="1">
+        <v>0</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>5</v>
@@ -4015,8 +4015,8 @@
       <c r="B181" s="0">
         <v>180</v>
       </c>
-      <c r="C181" s="1" t="s">
-        <v>5</v>
+      <c r="C181" s="1">
+        <v>0</v>
       </c>
       <c r="D181" s="0" t="s">
         <v>5</v>
@@ -4032,8 +4032,8 @@
       <c r="B182" s="0">
         <v>181</v>
       </c>
-      <c r="C182" s="1" t="s">
-        <v>5</v>
+      <c r="C182" s="1">
+        <v>0</v>
       </c>
       <c r="D182" s="0" t="s">
         <v>5</v>
@@ -4066,8 +4066,8 @@
       <c r="B184" s="0">
         <v>183</v>
       </c>
-      <c r="C184" s="1" t="s">
-        <v>5</v>
+      <c r="C184" s="1">
+        <v>0</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>5</v>
@@ -4100,8 +4100,8 @@
       <c r="B186" s="0">
         <v>185</v>
       </c>
-      <c r="C186" s="1" t="s">
-        <v>5</v>
+      <c r="C186" s="1">
+        <v>0</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>5</v>
@@ -4117,8 +4117,8 @@
       <c r="B187" s="0">
         <v>186</v>
       </c>
-      <c r="C187" s="1" t="s">
-        <v>5</v>
+      <c r="C187" s="1">
+        <v>0</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>5</v>
@@ -4134,8 +4134,8 @@
       <c r="B188" s="0">
         <v>187</v>
       </c>
-      <c r="C188" s="1" t="s">
-        <v>5</v>
+      <c r="C188" s="1">
+        <v>0</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>5</v>
@@ -4151,8 +4151,8 @@
       <c r="B189" s="0">
         <v>188</v>
       </c>
-      <c r="C189" s="1" t="s">
-        <v>5</v>
+      <c r="C189" s="1">
+        <v>0</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>5</v>
@@ -4168,8 +4168,8 @@
       <c r="B190" s="0">
         <v>189</v>
       </c>
-      <c r="C190" s="1" t="s">
-        <v>5</v>
+      <c r="C190" s="1">
+        <v>0</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>5</v>
@@ -4219,8 +4219,8 @@
       <c r="B193" s="0">
         <v>192</v>
       </c>
-      <c r="C193" s="1" t="s">
-        <v>5</v>
+      <c r="C193" s="1">
+        <v>0</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>5</v>
@@ -4236,8 +4236,8 @@
       <c r="B194" s="0">
         <v>193</v>
       </c>
-      <c r="C194" s="1" t="s">
-        <v>5</v>
+      <c r="C194" s="1">
+        <v>0</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>5</v>
@@ -4253,8 +4253,8 @@
       <c r="B195" s="0">
         <v>194</v>
       </c>
-      <c r="C195" s="1" t="s">
-        <v>5</v>
+      <c r="C195" s="1">
+        <v>0</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>5</v>
@@ -4287,8 +4287,8 @@
       <c r="B197" s="0">
         <v>196</v>
       </c>
-      <c r="C197" s="1" t="s">
-        <v>5</v>
+      <c r="C197" s="1">
+        <v>0</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>5</v>
@@ -4304,8 +4304,8 @@
       <c r="B198" s="0">
         <v>197</v>
       </c>
-      <c r="C198" s="1" t="s">
-        <v>5</v>
+      <c r="C198" s="1">
+        <v>0</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>5</v>
@@ -4321,8 +4321,8 @@
       <c r="B199" s="0">
         <v>198</v>
       </c>
-      <c r="C199" s="1" t="s">
-        <v>5</v>
+      <c r="C199" s="1">
+        <v>0</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>5</v>

</xml_diff>